<commit_message>
added data in row 2
</commit_message>
<xml_diff>
--- a/newexcel.xlsx
+++ b/newexcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\straw\Desktop\GitHub\intermediate_git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clifton/Dropbox/work/-/Git/intermediate_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B181CF9B-5738-4776-A915-546A9C0165BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814E8A9-E240-344C-8E2F-02CE9F67D065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7B3A4BC1-C635-4661-A007-949770963998}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="12560" xr2:uid="{7B3A4BC1-C635-4661-A007-949770963998}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -379,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC82D6AB-F0DD-4D29-9A19-8156A57EC315}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -402,6 +394,23 @@
       </c>
       <c r="E1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited excel, deleted file
</commit_message>
<xml_diff>
--- a/newexcel.xlsx
+++ b/newexcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clifton/Dropbox/work/-/Git/intermediate_git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\straw\Desktop\GitHub\intermediate_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814E8A9-E240-344C-8E2F-02CE9F67D065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06116C0E-FB8C-4B33-8837-C4AF2F78CB49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="12560" xr2:uid="{7B3A4BC1-C635-4661-A007-949770963998}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7B3A4BC1-C635-4661-A007-949770963998}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC82D6AB-F0DD-4D29-9A19-8156A57EC315}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>1</v>
       </c>
@@ -396,7 +413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>5</v>
       </c>
@@ -411,6 +428,20 @@
       </c>
       <c r="E2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>